<commit_message>
parse cal foreign spendings
</commit_message>
<xml_diff>
--- a/spendings/categories.xlsx
+++ b/spendings/categories.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3114" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3210" uniqueCount="1081">
   <si>
     <t xml:space="preserve">business_name</t>
   </si>
@@ -3173,6 +3173,96 @@
   </si>
   <si>
     <t xml:space="preserve">אלכסנדרה סינלניקוב</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חניון</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חניה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סופר מניה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">טיב טעם</t>
+  </si>
+  <si>
+    <t xml:space="preserve">דלק</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YELLOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מקדונלדס</t>
+  </si>
+  <si>
+    <t xml:space="preserve">קפה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">שופרסל</t>
+  </si>
+  <si>
+    <t xml:space="preserve">חניונים</t>
+  </si>
+  <si>
+    <t xml:space="preserve">משק 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PJ COSMETICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">זר פור יו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REGRUB RABTAEM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">אושר עד</t>
+  </si>
+  <si>
+    <t xml:space="preserve">קיי אס פי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מינימרקט אבו חסונה ובניו</t>
+  </si>
+  <si>
+    <t xml:space="preserve">לונה פארק</t>
+  </si>
+  <si>
+    <t xml:space="preserve">שילה- בר מסעדה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">תל אביב הילטון בעמ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">בייקרי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סופרפארם</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סופר אקספרס</t>
+  </si>
+  <si>
+    <t xml:space="preserve">עירית רמלה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">אולג בוליוק פרסום דיגיטלי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">היפר רוזנפלד</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סלקום</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מי עדן</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WIND</t>
   </si>
 </sst>
 </file>
@@ -3185,7 +3275,7 @@
     <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
     <numFmt numFmtId="167" formatCode="\€#,##0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -3222,6 +3312,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3266,7 +3362,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3304,6 +3400,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3384,10 +3484,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1045"/>
+  <dimension ref="A1:C1070"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1022" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1054" activeCellId="0" sqref="A1054"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14817,13 +14917,358 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1039" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1040" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1041" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1042" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1043" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1044" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1045" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1039" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1039" s="0" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B1039" s="0" t="s">
+        <v>831</v>
+      </c>
+      <c r="C1039" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1040" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1040" s="0" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B1040" s="0" t="s">
+        <v>831</v>
+      </c>
+      <c r="C1040" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1041" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1041" s="0" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B1041" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1041" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1042" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1042" s="0" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B1042" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1042" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1043" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1043" s="0" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B1043" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1043" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1044" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1044" s="0" t="s">
+        <v>454</v>
+      </c>
+      <c r="B1044" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1044" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1045" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1045" s="0" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B1045" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1045" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1046" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1046" s="0" t="s">
+        <v>585</v>
+      </c>
+      <c r="B1046" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1046" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1047" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1047" s="0" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B1047" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1047" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1048" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1048" s="0" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B1048" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1048" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1049" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1049" s="0" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B1049" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1049" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1050" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1050" s="0" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B1050" s="0" t="s">
+        <v>831</v>
+      </c>
+      <c r="C1050" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1051" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1051" s="0" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B1051" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1051" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1052" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1052" s="0" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B1052" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1052" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1053" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1053" s="0" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B1053" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1053" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1054" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1054" s="0" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B1054" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1054" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1055" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1055" s="0" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1055" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1055" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1056" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1056" s="10" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1056" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1056" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1057" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1057" s="0" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B1057" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1057" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1058" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1058" s="10" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1058" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1058" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1059" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1059" s="0" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B1059" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1059" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1060" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1060" s="0" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1060" s="0" t="s">
+        <v>831</v>
+      </c>
+      <c r="C1060" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1061" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1061" s="0" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1061" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1061" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1062" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1062" s="10" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B1062" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1062" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1063" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1063" s="10" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B1063" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1063" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1064" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1064" s="0" t="s">
+        <v>662</v>
+      </c>
+      <c r="B1064" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1064" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1065" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1065" s="0" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B1065" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1065" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1066" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1066" s="0" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1066" s="0" t="s">
+        <v>581</v>
+      </c>
+      <c r="C1066" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1067" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1067" s="0" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B1067" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1067" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1068" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1068" s="0" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B1068" s="0" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1068" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1069" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1069" s="10" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B1069" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1069" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="1070" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1070" s="0" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B1070" s="0" t="s">
+        <v>831</v>
+      </c>
+      <c r="C1070" s="0" t="s">
+        <v>1052</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A266" r:id="rId1" display="WWW.ALIEXPRESS.COM"/>

</xml_diff>